<commit_message>
preliminary event metrics fix
</commit_message>
<xml_diff>
--- a/Prelim_Data/High_Plains/High_Plains_30_90.xlsx
+++ b/Prelim_Data/High_Plains/High_Plains_30_90.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucdavis365-my.sharepoint.com/personal/aahernes_ucdavis_edu/Documents/WORK/DahlkeLab_LAWR/Prelim_Data/High_Plains/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_FE114ECB74D4899C27C4E2DB417AD59547121661" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ACCF5737-DB4C-4814-8F85-B137095F8DF0}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_FE114ECB74D4899C27C4E2DB417AD59547121661" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6CF03998-08CF-4373-A5CD-877C70358C36}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3243,6 +3243,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3532,13 +3536,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK328"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B90" sqref="B90"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="14" max="14" width="17" customWidth="1"/>
+    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="31" width="12" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
@@ -40610,6 +40636,7 @@
     <sortCondition ref="A2:A328"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>